<commit_message>
From 1.2.4 to 1.2.5 change and minor updates
</commit_message>
<xml_diff>
--- a/output/xlsx/UC002 - Gerenciar Diárias do Beneficiário (Minhas Diárias)--ART-.xlsx
+++ b/output/xlsx/UC002 - Gerenciar Diárias do Beneficiário (Minhas Diárias)--ART-.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Version: </t>
   </si>
   <si>
-    <t>1.0</t>
+    <t>1.2.5</t>
   </si>
   <si>
     <t>Suite Type:</t>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Precondition: </t>
   </si>
   <si>
-    <t>O usuario devidamente autenticado e na tela inicial do sistema</t>
+    <t>O usuário devidamente autenticado e na tela inicial do sistema.</t>
   </si>
   <si>
     <t>#</t>
@@ -104,7 +104,7 @@
     <t>Beneficiário Clica em detalhar diária.</t>
   </si>
   <si>
-    <t>SYSTEM Apresenta a tela de Detalhar Diárias</t>
+    <t>SYSTEM Apresenta a tela de Detalhar Diárias.</t>
   </si>
   <si>
     <t>TC3</t>
@@ -113,7 +113,7 @@
     <t>Beneficiário Clica em analisar prestação de contas.</t>
   </si>
   <si>
-    <t>SYSTEM Apresenta a tela de Analisar Prestação de Contas</t>
+    <t>SYSTEM Apresenta a tela de Analisar Prestação de Contas.</t>
   </si>
   <si>
     <t>TC4</t>
@@ -122,13 +122,13 @@
     <t>Beneficiário Clica em cancelar diária.</t>
   </si>
   <si>
-    <t>SYSTEM Apresenta a tela de Cancelar Solicitação de Diária</t>
+    <t>SYSTEM Apresenta a tela de Cancelar Solicitação de Diária.</t>
   </si>
   <si>
     <t>TC5</t>
   </si>
   <si>
-    <t>Beneficiário O usuario acessa o caso de uso atraves do menu.</t>
+    <t>Beneficiário Acessa o caso de uso através do menu.</t>
   </si>
   <si>
     <t>SYSTEM Apresenta a tela com a lista de diárias daquele beneficiário.</t>

</xml_diff>